<commit_message>
actualizado 27 de abril de 2020
</commit_message>
<xml_diff>
--- a/tbl/Reporte_Regional.xlsx
+++ b/tbl/Reporte_Regional.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luis\Documents\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luis\Documents\Desktop\RStudio\Git\Situacion-Covid19-por-Regiones-de-Chile\tbl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0678CA6E-E7A5-4BB2-8FF2-315D21CDD9C6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A766165-C0A8-4320-A293-12894FC03266}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="330" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -184,7 +184,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -201,13 +201,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -491,7 +485,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H37"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A18" sqref="A18"/>
@@ -541,27 +535,27 @@
         <v>4</v>
       </c>
       <c r="B2" s="2">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C2" s="2">
-        <v>170</v>
+        <v>265</v>
       </c>
       <c r="D2" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E2" s="2">
         <v>252110</v>
       </c>
       <c r="F2" s="3">
         <f>(C2/E2)*100000</f>
-        <v>67.430883344571811</v>
+        <v>105.11284756653842</v>
       </c>
       <c r="G2" s="3">
         <f>(D2/E2)*100000</f>
-        <v>0.79330450993613899</v>
-      </c>
-      <c r="H2" s="9">
-        <v>43942</v>
+        <v>1.1899567649042084</v>
+      </c>
+      <c r="H2" s="8">
+        <v>43948</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -569,27 +563,27 @@
         <v>10</v>
       </c>
       <c r="B3" s="2">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C3" s="2">
-        <v>104</v>
+        <v>164</v>
       </c>
       <c r="D3" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E3" s="2">
         <v>382773</v>
       </c>
       <c r="F3" s="3">
         <f t="shared" ref="F3:F17" si="0">(C3/E3)*100000</f>
-        <v>27.170150454708143</v>
+        <v>42.845237255501303</v>
       </c>
       <c r="G3" s="3">
-        <f t="shared" ref="G3:G17" si="1">(D3/E3)*100000</f>
-        <v>0</v>
-      </c>
-      <c r="H3" s="9">
-        <v>43942</v>
+        <f>(D3/E3)*100000</f>
+        <v>0.26125144667988598</v>
+      </c>
+      <c r="H3" s="8">
+        <v>43948</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -597,27 +591,27 @@
         <v>3</v>
       </c>
       <c r="B4" s="2">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="C4" s="2">
-        <v>291</v>
+        <v>457</v>
       </c>
       <c r="D4" s="2">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E4" s="2">
         <v>691854</v>
       </c>
       <c r="F4" s="3">
         <f t="shared" si="0"/>
-        <v>42.060897241325485</v>
+        <v>66.054398760432107</v>
       </c>
       <c r="G4" s="3">
-        <f t="shared" si="1"/>
-        <v>0.14453916577775081</v>
-      </c>
-      <c r="H4" s="9">
-        <v>43942</v>
+        <f t="shared" ref="G3:G17" si="1">(D4/E4)*100000</f>
+        <v>0.57815666311100322</v>
+      </c>
+      <c r="H4" s="8">
+        <v>43948</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -625,10 +619,10 @@
         <v>5</v>
       </c>
       <c r="B5" s="2">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C5" s="2">
-        <v>13</v>
+        <v>35</v>
       </c>
       <c r="D5" s="2">
         <v>0</v>
@@ -638,14 +632,14 @@
       </c>
       <c r="F5" s="3">
         <f t="shared" si="0"/>
-        <v>4.1308001995494248</v>
+        <v>11.121385152633067</v>
       </c>
       <c r="G5" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H5" s="9">
-        <v>43942</v>
+      <c r="H5" s="8">
+        <v>43948</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -653,10 +647,10 @@
         <v>6</v>
       </c>
       <c r="B6" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C6" s="2">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="D6" s="2">
         <v>0</v>
@@ -666,14 +660,14 @@
       </c>
       <c r="F6" s="3">
         <f t="shared" si="0"/>
-        <v>8.2526408450704221</v>
+        <v>8.8506582976117567</v>
       </c>
       <c r="G6" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H6" s="9">
-        <v>43942</v>
+      <c r="H6" s="8">
+        <v>43948</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -681,27 +675,27 @@
         <v>11</v>
       </c>
       <c r="B7" s="2">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="C7" s="2">
-        <v>403</v>
+        <v>485</v>
       </c>
       <c r="D7" s="2">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E7" s="2">
         <v>1960170</v>
       </c>
       <c r="F7" s="3">
         <f t="shared" si="0"/>
-        <v>20.559441272950814</v>
+        <v>24.74275190417158</v>
       </c>
       <c r="G7" s="3">
         <f t="shared" si="1"/>
-        <v>0.30609589984542157</v>
-      </c>
-      <c r="H7" s="9">
-        <v>43942</v>
+        <v>0.45914384976813238</v>
+      </c>
+      <c r="H7" s="8">
+        <v>43948</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -709,27 +703,27 @@
         <v>15</v>
       </c>
       <c r="B8" s="2">
-        <v>145</v>
+        <v>362</v>
       </c>
       <c r="C8" s="2">
-        <v>5788</v>
+        <v>7858</v>
       </c>
       <c r="D8" s="2">
-        <v>69</v>
+        <v>95</v>
       </c>
       <c r="E8" s="2">
         <v>8125072</v>
       </c>
       <c r="F8" s="3">
         <f t="shared" si="0"/>
-        <v>71.236291813783311</v>
+        <v>96.712989127973273</v>
       </c>
       <c r="G8" s="3">
         <f t="shared" si="1"/>
-        <v>0.84922324380633185</v>
-      </c>
-      <c r="H8" s="9">
-        <v>43942</v>
+        <v>1.1692204081391526</v>
+      </c>
+      <c r="H8" s="8">
+        <v>43948</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -737,10 +731,10 @@
         <v>16</v>
       </c>
       <c r="B9" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C9" s="2">
-        <v>57</v>
+        <v>94</v>
       </c>
       <c r="D9" s="2">
         <v>1</v>
@@ -750,14 +744,14 @@
       </c>
       <c r="F9" s="3">
         <f t="shared" si="0"/>
-        <v>5.7514002641608055</v>
+        <v>9.4847653479143101</v>
       </c>
       <c r="G9" s="3">
         <f t="shared" si="1"/>
         <v>0.10090175902036501</v>
       </c>
-      <c r="H9" s="9">
-        <v>43942</v>
+      <c r="H9" s="8">
+        <v>43948</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -765,27 +759,27 @@
         <v>9</v>
       </c>
       <c r="B10" s="2">
+        <v>9</v>
+      </c>
+      <c r="C10" s="2">
+        <v>363</v>
+      </c>
+      <c r="D10" s="2">
         <v>12</v>
-      </c>
-      <c r="C10" s="2">
-        <v>316</v>
-      </c>
-      <c r="D10" s="2">
-        <v>10</v>
       </c>
       <c r="E10" s="2">
         <v>1131939</v>
       </c>
       <c r="F10" s="3">
         <f t="shared" si="0"/>
-        <v>27.916698691360576</v>
+        <v>32.068865901784463</v>
       </c>
       <c r="G10" s="3">
         <f t="shared" si="1"/>
-        <v>0.88343983200508158</v>
-      </c>
-      <c r="H10" s="9">
-        <v>43942</v>
+        <v>1.0601277984060979</v>
+      </c>
+      <c r="H10" s="8">
+        <v>43948</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -793,27 +787,27 @@
         <v>12</v>
       </c>
       <c r="B11" s="2">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C11" s="2">
-        <v>694</v>
+        <v>741</v>
       </c>
       <c r="D11" s="2">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E11" s="2">
         <v>511551</v>
       </c>
       <c r="F11" s="3">
         <f t="shared" si="0"/>
-        <v>135.66584758899896</v>
+        <v>144.8535923104441</v>
       </c>
       <c r="G11" s="3">
         <f t="shared" si="1"/>
-        <v>2.5412910931656865</v>
-      </c>
-      <c r="H11" s="9">
-        <v>43942</v>
+        <v>2.736775023409201</v>
+      </c>
+      <c r="H11" s="8">
+        <v>43948</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -821,27 +815,27 @@
         <v>13</v>
       </c>
       <c r="B12" s="2">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="C12" s="2">
-        <v>636</v>
+        <v>706</v>
       </c>
       <c r="D12" s="2">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E12" s="2">
         <v>1663696</v>
       </c>
       <c r="F12" s="3">
         <f t="shared" si="0"/>
-        <v>38.228137832873315</v>
+        <v>42.435637279887672</v>
       </c>
       <c r="G12" s="3">
         <f t="shared" si="1"/>
-        <v>0.24042853982939189</v>
-      </c>
-      <c r="H12" s="9">
-        <v>43942</v>
+        <v>0.36064280974408786</v>
+      </c>
+      <c r="H12" s="8">
+        <v>43948</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -849,27 +843,27 @@
         <v>14</v>
       </c>
       <c r="B13" s="2">
-        <v>47</v>
+        <v>20</v>
       </c>
       <c r="C13" s="2">
-        <v>1092</v>
+        <v>1236</v>
       </c>
       <c r="D13" s="2">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="E13" s="2">
         <v>1014343</v>
       </c>
       <c r="F13" s="3">
         <f t="shared" si="0"/>
-        <v>107.65589154753373</v>
+        <v>121.8522728505052</v>
       </c>
       <c r="G13" s="3">
         <f t="shared" si="1"/>
-        <v>2.4646495317658821</v>
-      </c>
-      <c r="H13" s="9">
-        <v>43942</v>
+        <v>3.1547514006603286</v>
+      </c>
+      <c r="H13" s="8">
+        <v>43948</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -877,10 +871,10 @@
         <v>8</v>
       </c>
       <c r="B14" s="2">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C14" s="2">
-        <v>167</v>
+        <v>180</v>
       </c>
       <c r="D14" s="2">
         <v>3</v>
@@ -890,14 +884,14 @@
       </c>
       <c r="F14" s="3">
         <f t="shared" si="0"/>
-        <v>41.149728337871302</v>
+        <v>44.353000603693616</v>
       </c>
       <c r="G14" s="3">
         <f t="shared" si="1"/>
         <v>0.739216676728227</v>
       </c>
-      <c r="H14" s="9">
-        <v>43942</v>
+      <c r="H14" s="8">
+        <v>43948</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -905,27 +899,27 @@
         <v>7</v>
       </c>
       <c r="B15" s="2">
+        <v>4</v>
+      </c>
+      <c r="C15" s="2">
+        <v>477</v>
+      </c>
+      <c r="D15" s="2">
         <v>8</v>
-      </c>
-      <c r="C15" s="2">
-        <v>432</v>
-      </c>
-      <c r="D15" s="2">
-        <v>6</v>
       </c>
       <c r="E15" s="2">
         <v>891440</v>
       </c>
       <c r="F15" s="3">
         <f t="shared" si="0"/>
-        <v>48.460917167728617</v>
+        <v>53.508929372700351</v>
       </c>
       <c r="G15" s="3">
         <f t="shared" si="1"/>
-        <v>0.6730682939962308</v>
-      </c>
-      <c r="H15" s="9">
-        <v>43942</v>
+        <v>0.89742439199497437</v>
+      </c>
+      <c r="H15" s="8">
+        <v>43948</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -952,8 +946,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H16" s="9">
-        <v>43942</v>
+      <c r="H16" s="8">
+        <v>43948</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -961,44 +955,28 @@
         <v>18</v>
       </c>
       <c r="B17" s="2">
-        <v>27</v>
+        <v>3</v>
       </c>
       <c r="C17" s="2">
-        <v>593</v>
+        <v>671</v>
       </c>
       <c r="D17" s="2">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E17" s="2">
         <v>178362</v>
       </c>
       <c r="F17" s="3">
         <f t="shared" si="0"/>
-        <v>332.46992072302396</v>
+        <v>376.20120877765441</v>
       </c>
       <c r="G17" s="3">
         <f t="shared" si="1"/>
-        <v>3.9246027741335037</v>
-      </c>
-      <c r="H17" s="9">
-        <v>43942</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C26" s="8"/>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C27" s="8"/>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C31" s="8"/>
-    </row>
-    <row r="36" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C36" s="8"/>
-    </row>
-    <row r="37" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C37" s="8"/>
-      <c r="D37" s="10"/>
+        <v>5.6065753916192911</v>
+      </c>
+      <c r="H17" s="8">
+        <v>43948</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>

</xml_diff>